<commit_message>
created marts for each occupation field, updated schema.yml
</commit_message>
<xml_diff>
--- a/uppgiften/AI2_project_group.xlsx
+++ b/uppgiften/AI2_project_group.xlsx
@@ -300,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -327,10 +327,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -645,12 +648,12 @@
     <col min="3" max="3" style="9" width="36.14785714285715" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="9" width="29.719285714285714" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="9" width="36.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="28.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="36.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="28.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="36.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +677,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -698,7 +701,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -716,7 +719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
@@ -734,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
@@ -758,7 +761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -776,7 +779,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
@@ -794,7 +797,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -818,7 +821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
@@ -836,7 +839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -854,7 +857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -872,7 +875,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
       <c r="A12" s="7" t="s">
         <v>37</v>
       </c>
@@ -896,7 +899,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
@@ -914,7 +917,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
       <c r="A14" s="7" t="s">
         <v>44</v>
       </c>
@@ -932,7 +935,7 @@
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="7" t="s">
         <v>46</v>
       </c>
@@ -950,7 +953,7 @@
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="21">
       <c r="A16" s="4" t="s">
         <v>49</v>
       </c>
@@ -974,7 +977,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>

</xml_diff>